<commit_message>
fixed historic solar capacity additions and retirements
</commit_message>
<xml_diff>
--- a/data-extra/ira_comparison_raw/bistline-historic.xlsx
+++ b/data-extra/ira_comparison_raw/bistline-historic.xlsx
@@ -8,17 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\LEEP\data-extra\ira_comparison_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9708CF62-8FEF-4A72-91EC-64FEA3AF347D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FF6238-9774-4F81-98FA-4379B12FB053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="784" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="784" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ev share" sheetId="1" r:id="rId1"/>
     <sheet name="generation" sheetId="2" r:id="rId2"/>
-    <sheet name="capacity change" sheetId="3" r:id="rId3"/>
+    <sheet name="capacity change" sheetId="5" r:id="rId3"/>
     <sheet name="primary energy" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1043,13 +1056,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -1059,7 +1072,7 @@
     <col min="14" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1128,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1181,30 +1194,30 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1254,7 +1267,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1304,7 +1317,7 @@
         <v>334087.60100000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1354,7 +1367,7 @@
         <v>375298.35499999998</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1404,7 +1417,7 @@
         <v>403829.413</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1454,7 +1467,7 @@
         <v>447048.56300000002</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1504,7 +1517,7 @@
         <v>476257.61800000002</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1554,7 +1567,7 @@
         <v>550298.86199999996</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1604,7 +1617,7 @@
         <v>603875.76300000004</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1654,7 +1667,7 @@
         <v>634642.36699999997</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1704,7 +1717,7 @@
         <v>648450.86199999996</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1754,7 +1767,7 @@
         <v>713378.83100000001</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1804,7 +1817,7 @@
         <v>759155.78799999994</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1854,7 +1867,7 @@
         <v>797124.39099999995</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1904,7 +1917,7 @@
         <v>857943.65599999996</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1954,7 +1967,7 @@
         <v>920028.27099999995</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -2004,7 +2017,7 @@
         <v>987218.326</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2054,7 +2067,7 @@
         <v>1058385.6710000001</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -2104,7 +2117,7 @@
         <v>1147531.895</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -2154,7 +2167,7 @@
         <v>1217795.6880000001</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2204,7 +2217,7 @@
         <v>1332825.601</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2254,7 +2267,7 @@
         <v>1445458.0560000001</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2304,7 +2317,7 @@
         <v>1535111.4669999999</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -2354,7 +2367,7 @@
         <v>1615853.6159999999</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2404,7 +2417,7 @@
         <v>1752978.4129999999</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2454,7 +2467,7 @@
         <v>1864056.632</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -2504,7 +2517,7 @@
         <v>1870319.4040000001</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2554,7 +2567,7 @@
         <v>1920754.5689999999</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -2604,7 +2617,7 @@
         <v>2040913.6810000001</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2654,7 +2667,7 @@
         <v>2127447.4879999999</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -2704,7 +2717,7 @@
         <v>2209376.9109999998</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -2754,7 +2767,7 @@
         <v>2250665.0249999999</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>23</v>
       </c>
@@ -2804,7 +2817,7 @@
         <v>2289600.3640000001</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -2854,7 +2867,7 @@
         <v>2297973.338</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -2904,7 +2917,7 @@
         <v>2244372.4870000002</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -2954,7 +2967,7 @@
         <v>2313445.6860000002</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -3004,7 +3017,7 @@
         <v>2419465.3670000001</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>23</v>
       </c>
@@ -3054,7 +3067,7 @@
         <v>2473002.12</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -3104,7 +3117,7 @@
         <v>2490470.952</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -3154,7 +3167,7 @@
         <v>2575287.6669999999</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -3204,7 +3217,7 @@
         <v>2707411.1779999998</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -3254,7 +3267,7 @@
         <v>2967146.0869999998</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -3304,7 +3317,7 @@
         <v>3037827.3369999998</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -3354,7 +3367,7 @@
         <v>3073798.8849999998</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -3404,7 +3417,7 @@
         <v>3083882.2039999999</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -3454,7 +3467,7 @@
         <v>3197191.0959999999</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3517,7 @@
         <v>3247522.3879999998</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -3554,7 +3567,7 @@
         <v>3353487.3620000002</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>23</v>
       </c>
@@ -3604,7 +3617,7 @@
         <v>3444187.6209999998</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>23</v>
       </c>
@@ -3654,7 +3667,7 @@
         <v>3492172.2829999998</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>23</v>
       </c>
@@ -3704,7 +3717,7 @@
         <v>3620295.4980000001</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>23</v>
       </c>
@@ -3754,7 +3767,7 @@
         <v>3694809.81</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>23</v>
       </c>
@@ -3804,7 +3817,7 @@
         <v>3802105.0430000001</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -3854,7 +3867,7 @@
         <v>3736643.6490000002</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -3904,7 +3917,7 @@
         <v>3858452.2459999998</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>23</v>
       </c>
@@ -3954,7 +3967,7 @@
         <v>3883185.2039999999</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -4004,7 +4017,7 @@
         <v>3970555.264</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>23</v>
       </c>
@@ -4054,7 +4067,7 @@
         <v>4055422.75</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>23</v>
       </c>
@@ -4104,7 +4117,7 @@
         <v>4064702.2280000001</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>23</v>
       </c>
@@ -4154,7 +4167,7 @@
         <v>4156744.7239999999</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>23</v>
       </c>
@@ -4204,7 +4217,7 @@
         <v>4119387.76</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -4254,7 +4267,7 @@
         <v>3950330.9270000001</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>23</v>
       </c>
@@ -4304,7 +4317,7 @@
         <v>4125059.9</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>23</v>
       </c>
@@ -4354,7 +4367,7 @@
         <v>4100140.9270000001</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -4404,7 +4417,7 @@
         <v>4047765.26</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>23</v>
       </c>
@@ -4454,7 +4467,7 @@
         <v>4065964.068</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -4504,7 +4517,7 @@
         <v>4093564.1430000002</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>23</v>
       </c>
@@ -4554,7 +4567,7 @@
         <v>4078713.773</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>23</v>
       </c>
@@ -4604,7 +4617,7 @@
         <v>4077573.801</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -4654,7 +4667,7 @@
         <v>4035442.895</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -4704,7 +4717,7 @@
         <v>4180987.7030000002</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>23</v>
       </c>
@@ -4754,7 +4767,7 @@
         <v>4130573.88</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>23</v>
       </c>
@@ -4804,7 +4817,7 @@
         <v>4009766.8459999999</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>23</v>
       </c>
@@ -4860,45 +4873,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:BY18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7925B851-2F36-494D-96DA-D0E31235A7B1}">
+  <dimension ref="A1:BX18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="23" width="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="29" width="8" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="8" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" bestFit="1" customWidth="1"/>
-    <col min="40" max="54" width="7" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="8" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7" bestFit="1" customWidth="1"/>
-    <col min="57" max="60" width="8" bestFit="1" customWidth="1"/>
-    <col min="61" max="65" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="8" bestFit="1" customWidth="1"/>
-    <col min="73" max="75" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -5127,11 +5117,8 @@
       <c r="BX1">
         <v>2021</v>
       </c>
-      <c r="BY1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5360,11 +5347,8 @@
       <c r="BX2">
         <v>6.8704000000000001</v>
       </c>
-      <c r="BY2">
-        <v>9.1941000000000006</v>
-      </c>
-    </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5453,7 +5437,7 @@
         <v>1.1639999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5682,11 +5666,8 @@
       <c r="BX4">
         <v>4.7699999999999999E-2</v>
       </c>
-      <c r="BY4">
-        <v>7.8799999999999995E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -5822,11 +5803,8 @@
       <c r="BX5">
         <v>14.2818</v>
       </c>
-      <c r="BY5">
-        <v>11.189399999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -6055,11 +6033,8 @@
       <c r="BX6">
         <v>8.9700000000000002E-2</v>
       </c>
-      <c r="BY6">
-        <v>6.8599999999999994E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6271,7 +6246,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6387,25 +6362,25 @@
         <v>0</v>
       </c>
       <c r="AM8">
-        <v>0</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="AN8">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="AO8">
-        <v>0</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="AP8">
-        <v>0</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AQ8">
-        <v>0</v>
+        <v>7.2400000000000006E-2</v>
       </c>
       <c r="AR8">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="AS8">
-        <v>0</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AT8">
         <v>0</v>
@@ -6429,82 +6404,79 @@
         <v>0</v>
       </c>
       <c r="BA8">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="BB8">
-        <v>0</v>
+        <v>1E-4</v>
       </c>
       <c r="BC8">
         <v>0</v>
       </c>
       <c r="BD8">
-        <v>0</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="BE8">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="BF8">
-        <v>0</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="BG8">
         <v>0</v>
       </c>
       <c r="BH8">
-        <v>0</v>
+        <v>2.8E-3</v>
       </c>
       <c r="BI8">
-        <v>0</v>
+        <v>1.8E-3</v>
       </c>
       <c r="BJ8">
-        <v>0</v>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="BK8">
-        <v>0</v>
+        <v>3.2899999999999999E-2</v>
       </c>
       <c r="BL8">
-        <v>0</v>
+        <v>0.1069</v>
       </c>
       <c r="BM8">
-        <v>0</v>
+        <v>0.23130000000000001</v>
       </c>
       <c r="BN8">
-        <v>0</v>
+        <v>0.77800000000000002</v>
       </c>
       <c r="BO8">
-        <v>0</v>
+        <v>1.6085</v>
       </c>
       <c r="BP8">
-        <v>0</v>
+        <v>3.5373999999999999</v>
       </c>
       <c r="BQ8">
-        <v>0</v>
+        <v>3.6644999999999999</v>
       </c>
       <c r="BR8">
-        <v>0</v>
+        <v>5.9209999999999994</v>
       </c>
       <c r="BS8">
-        <v>0</v>
+        <v>10.8818</v>
       </c>
       <c r="BT8">
-        <v>0</v>
+        <v>8.4903999999999993</v>
       </c>
       <c r="BU8">
-        <v>0</v>
+        <v>8.2860000000000014</v>
       </c>
       <c r="BV8">
-        <v>0</v>
+        <v>9.2073</v>
       </c>
       <c r="BW8">
-        <v>0</v>
+        <v>14.939699999999997</v>
       </c>
       <c r="BX8">
-        <v>0</v>
-      </c>
-      <c r="BY8">
-        <v>17.771000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+        <v>18.6065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -6568,11 +6540,8 @@
       <c r="BX9">
         <v>3.2244999999999999</v>
       </c>
-      <c r="BY9">
-        <v>6.1791999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6586,7 +6555,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -6659,11 +6628,8 @@
       <c r="BX11">
         <v>-0.95379999999999998</v>
       </c>
-      <c r="BY11">
-        <v>-1.0931</v>
-      </c>
-    </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -6697,11 +6663,8 @@
       <c r="BX12">
         <v>-1.0394000000000001</v>
       </c>
-      <c r="BY12">
-        <v>-0.76849999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -6774,11 +6737,8 @@
       <c r="BX13">
         <v>-0.93140000000000001</v>
       </c>
-      <c r="BY13">
-        <v>-0.28810000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -6849,7 +6809,7 @@
         <v>-0.23430000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -6923,7 +6883,7 @@
         <v>-8.8000000000000005E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -6996,11 +6956,8 @@
       <c r="BX16">
         <v>-5.5723000000000003</v>
       </c>
-      <c r="BY16">
-        <v>-6.6502999999999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:76" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -7038,7 +6995,7 @@
         <v>-0.27</v>
       </c>
     </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:76" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -7085,18 +7042,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -7113,7 +7070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1949</v>
       </c>
@@ -7130,7 +7087,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1950</v>
       </c>
@@ -7147,7 +7104,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1951</v>
       </c>
@@ -7164,7 +7121,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1952</v>
       </c>
@@ -7181,7 +7138,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>1953</v>
       </c>
@@ -7198,7 +7155,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1954</v>
       </c>
@@ -7215,7 +7172,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1955</v>
       </c>
@@ -7232,7 +7189,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>1956</v>
       </c>
@@ -7249,7 +7206,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>1957</v>
       </c>
@@ -7266,7 +7223,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>1958</v>
       </c>
@@ -7283,7 +7240,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>1959</v>
       </c>
@@ -7300,7 +7257,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>1960</v>
       </c>
@@ -7317,7 +7274,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>1961</v>
       </c>
@@ -7334,7 +7291,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>1962</v>
       </c>
@@ -7351,7 +7308,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>1963</v>
       </c>
@@ -7368,7 +7325,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>1964</v>
       </c>
@@ -7385,7 +7342,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>1965</v>
       </c>
@@ -7402,7 +7359,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>1966</v>
       </c>
@@ -7419,7 +7376,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>1967</v>
       </c>
@@ -7436,7 +7393,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>1968</v>
       </c>
@@ -7453,7 +7410,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>1969</v>
       </c>
@@ -7470,7 +7427,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>1970</v>
       </c>
@@ -7487,7 +7444,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>1971</v>
       </c>
@@ -7504,7 +7461,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>1972</v>
       </c>
@@ -7521,7 +7478,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>1973</v>
       </c>
@@ -7538,7 +7495,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>1974</v>
       </c>
@@ -7555,7 +7512,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>1975</v>
       </c>
@@ -7572,7 +7529,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>1976</v>
       </c>
@@ -7589,7 +7546,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>1977</v>
       </c>
@@ -7606,7 +7563,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>1978</v>
       </c>
@@ -7623,7 +7580,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>1979</v>
       </c>
@@ -7640,7 +7597,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>1980</v>
       </c>
@@ -7657,7 +7614,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>1981</v>
       </c>
@@ -7674,7 +7631,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>1982</v>
       </c>
@@ -7691,7 +7648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>1983</v>
       </c>
@@ -7708,7 +7665,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>1984</v>
       </c>
@@ -7725,7 +7682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>1985</v>
       </c>
@@ -7742,7 +7699,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>1986</v>
       </c>
@@ -7759,7 +7716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>1987</v>
       </c>
@@ -7776,7 +7733,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>1988</v>
       </c>
@@ -7793,7 +7750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>1989</v>
       </c>
@@ -7810,7 +7767,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>1990</v>
       </c>
@@ -7827,7 +7784,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>1991</v>
       </c>
@@ -7844,7 +7801,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>1992</v>
       </c>
@@ -7861,7 +7818,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>1993</v>
       </c>
@@ -7878,7 +7835,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>1994</v>
       </c>
@@ -7895,7 +7852,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>1995</v>
       </c>
@@ -7912,7 +7869,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>1996</v>
       </c>
@@ -7929,7 +7886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>1997</v>
       </c>
@@ -7946,7 +7903,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>1998</v>
       </c>
@@ -7963,7 +7920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>1999</v>
       </c>
@@ -7980,7 +7937,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>2000</v>
       </c>
@@ -7997,7 +7954,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>2001</v>
       </c>
@@ -8014,7 +7971,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>2002</v>
       </c>
@@ -8031,7 +7988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>2003</v>
       </c>
@@ -8048,7 +8005,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>2004</v>
       </c>
@@ -8065,7 +8022,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>2005</v>
       </c>
@@ -8082,7 +8039,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>2006</v>
       </c>
@@ -8099,7 +8056,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>2007</v>
       </c>
@@ -8116,7 +8073,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>2008</v>
       </c>
@@ -8133,7 +8090,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>2009</v>
       </c>
@@ -8150,7 +8107,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>2010</v>
       </c>
@@ -8167,7 +8124,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>2011</v>
       </c>
@@ -8184,7 +8141,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>2012</v>
       </c>
@@ -8201,7 +8158,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>2013</v>
       </c>
@@ -8218,7 +8175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>2014</v>
       </c>
@@ -8235,7 +8192,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>2015</v>
       </c>
@@ -8252,7 +8209,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>2016</v>
       </c>
@@ -8269,7 +8226,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>2017</v>
       </c>
@@ -8286,7 +8243,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>2018</v>
       </c>
@@ -8303,7 +8260,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>2019</v>
       </c>
@@ -8320,7 +8277,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>2020</v>
       </c>
@@ -8337,7 +8294,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>2021</v>
       </c>

</xml_diff>